<commit_message>
adding variable types nominal/ordinal
</commit_message>
<xml_diff>
--- a/Schema.xlsx
+++ b/Schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\Proyectos GitHub\SoftwareReuse_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luisa Restrepo\Desktop\Proyectos GitHub\SoftwareReuse_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497D33BF-A09D-4EF1-91D9-494FC8EEF70C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B86520F-D233-4DFF-9A0D-251362994465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="703" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="600" windowWidth="13695" windowHeight="10920" tabRatio="703" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schema" sheetId="8" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="666">
   <si>
     <t>respondent_id</t>
   </si>
@@ -2024,6 +2023,15 @@
   </si>
   <si>
     <t>Associated Research Question</t>
+  </si>
+  <si>
+    <t>Variable Type</t>
+  </si>
+  <si>
+    <t>Ordinal</t>
+  </si>
+  <si>
+    <t>Nominal</t>
   </si>
 </sst>
 </file>
@@ -2328,7 +2336,16 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2624,57 +2641,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:E58" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A1:E58" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table4" displayName="Table4" ref="A1:F58" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A1:F58" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F58">
     <sortCondition ref="A1:A58"/>
   </sortState>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Question Identifier" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Question type" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Question Spanish" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{82937DDA-D9FC-4287-921B-A1AF2D7B4719}" name="Question English" dataDxfId="17"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Answers options" dataDxfId="16"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Question Identifier" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Question type" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Question Spanish" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{82937DDA-D9FC-4287-921B-A1AF2D7B4719}" name="Question English" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{28CB06A4-EE87-47DD-91CD-F6A69177AAF4}" name="Variable Type" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Answers options" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="A1:E143" totalsRowShown="0" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table5" displayName="Table5" ref="A1:E143" totalsRowShown="0" tableBorderDxfId="16">
   <autoFilter ref="A1:E143" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D143">
     <sortCondition ref="A1:A143"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="#" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{C0E89F5C-EC9D-4EC0-A0E6-94D32E390030}" name="Question Identifier" dataDxfId="13"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Answer Identifier" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="ANSWER SPANISH" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{5A70E9DB-C552-4874-BE47-34EDAAEDDD92}" name="ANSWER ENGLISH" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="#" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{C0E89F5C-EC9D-4EC0-A0E6-94D32E390030}" name="Question Identifier" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Answer Identifier" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="ANSWER SPANISH" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{5A70E9DB-C552-4874-BE47-34EDAAEDDD92}" name="ANSWER ENGLISH" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table2" displayName="Table2" ref="A2:G56" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table2" displayName="Table2" ref="A2:G56" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A2:G56" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:G56">
     <sortCondition ref="G2:G56"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Dimension" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{58064347-6C0F-49BF-82E0-D7BB70900D52}" name="Column1" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Dimension" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{58064347-6C0F-49BF-82E0-D7BB70900D52}" name="Column1" dataDxfId="7">
       <calculatedColumnFormula>+CONCATENATE(Table2[[#This Row],[Factor]],Table2[[#This Row],[Question Identifier]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Factor" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Orden" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Question Identifier" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Question" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Factor" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Orden" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="Question Identifier" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Question" dataDxfId="3">
       <calculatedColumnFormula>+VLOOKUP(Table2[[#This Row],[Question Identifier]],Table4[[Question Identifier]:[Question English]],4,)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{88E61EA0-31C1-40F1-9E3A-FF520DEDA63B}" name="Associated Research Question" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{88E61EA0-31C1-40F1-9E3A-FF520DEDA63B}" name="Associated Research Question" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2685,7 +2703,7 @@
   <autoFilter ref="A1:C9" xr:uid="{D135F127-0B74-43D8-B995-75C65C50232E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{F9B95BF4-B40B-4F50-B485-EB192145AFFF}" name="Question Identifier"/>
-    <tableColumn id="4" xr3:uid="{6F1BA106-045C-4081-B97A-B11DC398A6FA}" name="Categories created Spanish" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{6F1BA106-045C-4081-B97A-B11DC398A6FA}" name="Categories created Spanish" dataDxfId="1">
       <calculatedColumnFormula>+CONCATENATE(B14:F14)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{7996DAD0-94CC-4AEB-B84A-82A7711A0D7D}" name="Categories created English"/>
@@ -2979,10 +2997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2990,12 +3008,13 @@
     <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="92.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="36.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>485</v>
       </c>
@@ -3009,10 +3028,13 @@
         <v>490</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
         <v>10</v>
       </c>
@@ -3025,9 +3047,12 @@
       <c r="D2" s="14" t="s">
         <v>491</v>
       </c>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
         <v>11</v>
       </c>
@@ -3040,9 +3065,12 @@
       <c r="D3" s="14" t="s">
         <v>492</v>
       </c>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
         <v>12</v>
       </c>
@@ -3055,9 +3083,12 @@
       <c r="D4" s="14" t="s">
         <v>493</v>
       </c>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>255</v>
       </c>
@@ -3070,9 +3101,12 @@
       <c r="D5" s="14" t="s">
         <v>494</v>
       </c>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="28" t="s">
         <v>42</v>
       </c>
@@ -3085,11 +3119,14 @@
       <c r="D6" s="14" t="s">
         <v>495</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F6" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
         <v>43</v>
       </c>
@@ -3102,11 +3139,14 @@
       <c r="D7" s="14" t="s">
         <v>496</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F7" s="14">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>44</v>
       </c>
@@ -3119,11 +3159,14 @@
       <c r="D8" s="14" t="s">
         <v>497</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F8" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>45</v>
       </c>
@@ -3136,11 +3179,14 @@
       <c r="D9" s="14" t="s">
         <v>498</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F9" s="14">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>58</v>
       </c>
@@ -3153,8 +3199,11 @@
       <c r="D10" s="14" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="14" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
         <v>65</v>
       </c>
@@ -3167,9 +3216,12 @@
       <c r="D11" s="14" t="s">
         <v>446</v>
       </c>
-      <c r="E11" s="14"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
         <v>59</v>
       </c>
@@ -3182,9 +3234,12 @@
       <c r="D12" s="14" t="s">
         <v>499</v>
       </c>
-      <c r="E12" s="14"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>15</v>
       </c>
@@ -3197,11 +3252,14 @@
       <c r="D13" s="14" t="s">
         <v>500</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F13" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>16</v>
       </c>
@@ -3214,11 +3272,14 @@
       <c r="D14" s="14" t="s">
         <v>501</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F14" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>17</v>
       </c>
@@ -3231,11 +3292,14 @@
       <c r="D15" s="14" t="s">
         <v>502</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F15" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
         <v>18</v>
       </c>
@@ -3248,11 +3312,14 @@
       <c r="D16" s="14" t="s">
         <v>503</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F16" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
         <v>19</v>
       </c>
@@ -3265,11 +3332,14 @@
       <c r="D17" s="14" t="s">
         <v>504</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F17" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>20</v>
       </c>
@@ -3282,11 +3352,14 @@
       <c r="D18" s="14" t="s">
         <v>505</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F18" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
         <v>21</v>
       </c>
@@ -3299,11 +3372,14 @@
       <c r="D19" s="14" t="s">
         <v>506</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F19" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
         <v>22</v>
       </c>
@@ -3316,11 +3392,14 @@
       <c r="D20" s="14" t="s">
         <v>507</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F20" s="14">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
         <v>66</v>
       </c>
@@ -3333,9 +3412,12 @@
       <c r="D21" s="14" t="s">
         <v>508</v>
       </c>
-      <c r="E21" s="14"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
         <v>46</v>
       </c>
@@ -3348,11 +3430,14 @@
       <c r="D22" s="14" t="s">
         <v>509</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F22" s="14">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
         <v>36</v>
       </c>
@@ -3365,11 +3450,14 @@
       <c r="D23" s="14" t="s">
         <v>510</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F23" s="14">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
         <v>47</v>
       </c>
@@ -3382,11 +3470,14 @@
       <c r="D24" s="14" t="s">
         <v>511</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F24" s="14">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>48</v>
       </c>
@@ -3399,11 +3490,14 @@
       <c r="D25" s="14" t="s">
         <v>512</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F25" s="14">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
         <v>23</v>
       </c>
@@ -3416,11 +3510,14 @@
       <c r="D26" s="14" t="s">
         <v>513</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F26" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>24</v>
       </c>
@@ -3433,11 +3530,14 @@
       <c r="D27" s="14" t="s">
         <v>514</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F27" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
         <v>25</v>
       </c>
@@ -3450,11 +3550,14 @@
       <c r="D28" s="14" t="s">
         <v>515</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F28" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
         <v>26</v>
       </c>
@@ -3467,11 +3570,14 @@
       <c r="D29" s="14" t="s">
         <v>516</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F29" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
         <v>27</v>
       </c>
@@ -3484,11 +3590,14 @@
       <c r="D30" s="14" t="s">
         <v>517</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F30" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>28</v>
       </c>
@@ -3501,11 +3610,14 @@
       <c r="D31" s="14" t="s">
         <v>518</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F31" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
         <v>29</v>
       </c>
@@ -3518,11 +3630,14 @@
       <c r="D32" s="14" t="s">
         <v>612</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F32" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
         <v>49</v>
       </c>
@@ -3535,11 +3650,14 @@
       <c r="D33" s="14" t="s">
         <v>519</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F33" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
         <v>467</v>
       </c>
@@ -3552,11 +3670,14 @@
       <c r="D34" s="14" t="s">
         <v>520</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F34" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
         <v>468</v>
       </c>
@@ -3569,11 +3690,14 @@
       <c r="D35" s="14" t="s">
         <v>521</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F35" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>51</v>
       </c>
@@ -3586,11 +3710,14 @@
       <c r="D36" s="14" t="s">
         <v>522</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F36" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>30</v>
       </c>
@@ -3603,11 +3730,14 @@
       <c r="D37" s="14" t="s">
         <v>523</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F37" s="14">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
         <v>60</v>
       </c>
@@ -3620,9 +3750,12 @@
       <c r="D38" s="14" t="s">
         <v>524</v>
       </c>
-      <c r="E38" s="14"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
         <v>31</v>
       </c>
@@ -3635,11 +3768,14 @@
       <c r="D39" s="14" t="s">
         <v>525</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E39" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F39" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>32</v>
       </c>
@@ -3652,11 +3788,14 @@
       <c r="D40" s="14" t="s">
         <v>526</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F40" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>61</v>
       </c>
@@ -3669,9 +3808,12 @@
       <c r="D41" s="14" t="s">
         <v>527</v>
       </c>
-      <c r="E41" s="14"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F41" s="14"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
         <v>13</v>
       </c>
@@ -3684,11 +3826,14 @@
       <c r="D42" s="14" t="s">
         <v>528</v>
       </c>
-      <c r="E42" s="14">
+      <c r="E42" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F42" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>52</v>
       </c>
@@ -3701,11 +3846,14 @@
       <c r="D43" s="14" t="s">
         <v>529</v>
       </c>
-      <c r="E43" s="14">
+      <c r="E43" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F43" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
         <v>33</v>
       </c>
@@ -3718,11 +3866,14 @@
       <c r="D44" s="14" t="s">
         <v>530</v>
       </c>
-      <c r="E44" s="14">
+      <c r="E44" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F44" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>34</v>
       </c>
@@ -3735,11 +3886,14 @@
       <c r="D45" s="14" t="s">
         <v>531</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F45" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
         <v>35</v>
       </c>
@@ -3752,11 +3906,14 @@
       <c r="D46" s="14" t="s">
         <v>532</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E46" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="F46" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
         <v>53</v>
       </c>
@@ -3769,11 +3926,14 @@
       <c r="D47" s="14" t="s">
         <v>635</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F47" s="14">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="28" t="s">
         <v>54</v>
       </c>
@@ -3786,11 +3946,14 @@
       <c r="D48" s="14" t="s">
         <v>533</v>
       </c>
-      <c r="E48" s="14">
+      <c r="E48" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F48" s="14">
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
         <v>55</v>
       </c>
@@ -3803,11 +3966,14 @@
       <c r="D49" s="14" t="s">
         <v>534</v>
       </c>
-      <c r="E49" s="14">
+      <c r="E49" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F49" s="14">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>56</v>
       </c>
@@ -3820,9 +3986,12 @@
       <c r="D50" s="14" t="s">
         <v>535</v>
       </c>
-      <c r="E50" s="14"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F50" s="14"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>37</v>
       </c>
@@ -3835,11 +4004,14 @@
       <c r="D51" s="14" t="s">
         <v>536</v>
       </c>
-      <c r="E51" s="14">
+      <c r="E51" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F51" s="14">
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>38</v>
       </c>
@@ -3852,11 +4024,14 @@
       <c r="D52" s="14" t="s">
         <v>537</v>
       </c>
-      <c r="E52" s="14">
+      <c r="E52" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F52" s="14">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>39</v>
       </c>
@@ -3869,11 +4044,14 @@
       <c r="D53" s="14" t="s">
         <v>538</v>
       </c>
-      <c r="E53" s="14">
+      <c r="E53" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F53" s="14">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
         <v>40</v>
       </c>
@@ -3886,11 +4064,14 @@
       <c r="D54" s="14" t="s">
         <v>539</v>
       </c>
-      <c r="E54" s="14">
+      <c r="E54" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F54" s="14">
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
         <v>14</v>
       </c>
@@ -3903,9 +4084,12 @@
       <c r="D55" s="14" t="s">
         <v>625</v>
       </c>
-      <c r="E55" s="14"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F55" s="14"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
         <v>41</v>
       </c>
@@ -3918,11 +4102,14 @@
       <c r="D56" s="14" t="s">
         <v>540</v>
       </c>
-      <c r="E56" s="14">
+      <c r="E56" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F56" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
         <v>0</v>
       </c>
@@ -3935,9 +4122,12 @@
       <c r="D57" s="14" t="s">
         <v>259</v>
       </c>
-      <c r="E57" s="14"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F57" s="14"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
         <v>9</v>
       </c>
@@ -3950,7 +4140,10 @@
       <c r="D58" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="14"/>
+      <c r="E58" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="F58" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3966,7 +4159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
@@ -6708,7 +6901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:BY59"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>